<commit_message>
CIC 874 Project - Got most of Part C write-up done, committing before generating more results on work computer
</commit_message>
<xml_diff>
--- a/CISC874/Project/Data/NetworkPerformance.xlsx
+++ b/CISC874/Project/Data/NetworkPerformance.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -290,7 +290,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FE4B-4509-83CC-5EFBCF618029}"/>
             </c:ext>
@@ -304,11 +304,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="307171880"/>
-        <c:axId val="307172536"/>
+        <c:axId val="163149656"/>
+        <c:axId val="163147696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="307171880"/>
+        <c:axId val="163149656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -365,12 +365,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="307172536"/>
+        <c:crossAx val="163147696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="307172536"/>
+        <c:axId val="163147696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -427,7 +427,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="307171880"/>
+        <c:crossAx val="163149656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1332,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L32" workbookViewId="0">
-      <selection activeCell="T69" sqref="T69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P63" sqref="P63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2162,7 +2162,7 @@
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1">
-        <f t="shared" ref="J42:Y42" si="1">AVERAGE(K16:K25)</f>
+        <f t="shared" ref="K42:Y42" si="1">AVERAGE(K16:K25)</f>
         <v>1.0231905139153901E-3</v>
       </c>
       <c r="L42" s="1">
@@ -2242,7 +2242,7 @@
         <v>4.0854877981869511E-3</v>
       </c>
       <c r="K43">
-        <f t="shared" ref="J43:Y43" si="3">_xlfn.STDEV.S(K16:K25)</f>
+        <f t="shared" ref="K43:Y43" si="3">_xlfn.STDEV.S(K16:K25)</f>
         <v>1.2270956469753742E-3</v>
       </c>
       <c r="L43">
@@ -2319,7 +2319,7 @@
         <v>0.15410573999999999</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" ref="D47:F47" si="4">D16*180</f>
+        <f t="shared" ref="D47:E47" si="4">D16*180</f>
         <v>1.1627334</v>
       </c>
       <c r="E47" s="1">
@@ -2354,7 +2354,7 @@
       </c>
       <c r="N47" s="1"/>
       <c r="O47" s="1">
-        <f t="shared" ref="N47:W47" si="7">O16*180</f>
+        <f t="shared" ref="O47:S47" si="7">O16*180</f>
         <v>1.4536907999999999</v>
       </c>
       <c r="P47" s="1">
@@ -2410,7 +2410,7 @@
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1">
-        <f t="shared" ref="F48:L48" si="12">G17*180</f>
+        <f t="shared" ref="G48:L48" si="12">G17*180</f>
         <v>0.64060019999999995</v>
       </c>
       <c r="H48" s="1">
@@ -2436,7 +2436,7 @@
       </c>
       <c r="N48" s="1"/>
       <c r="O48" s="1">
-        <f t="shared" ref="N48:W48" si="14">O17*180</f>
+        <f t="shared" ref="O48:S48" si="14">O17*180</f>
         <v>0.20832299999999998</v>
       </c>
       <c r="P48" s="1">
@@ -2457,7 +2457,7 @@
         <v>3.9816000000000003</v>
       </c>
       <c r="U48" s="1">
-        <f t="shared" ref="U48:Z48" si="16">U17*180</f>
+        <f t="shared" ref="U48:W48" si="16">U17*180</f>
         <v>4.0987079999999994</v>
       </c>
       <c r="V48" s="1"/>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1">
-        <f t="shared" ref="F49:L49" si="18">G18*180</f>
+        <f t="shared" ref="G49:L49" si="18">G18*180</f>
         <v>0.2579436</v>
       </c>
       <c r="H49" s="1">
@@ -2518,7 +2518,7 @@
       </c>
       <c r="N49" s="1"/>
       <c r="O49" s="1">
-        <f t="shared" ref="N49:W49" si="20">O18*180</f>
+        <f t="shared" ref="O49:S49" si="20">O18*180</f>
         <v>8.2439279999999995E-10</v>
       </c>
       <c r="P49" s="1">
@@ -2539,7 +2539,7 @@
         <v>1.573083</v>
       </c>
       <c r="U49" s="1">
-        <f t="shared" ref="U49:Z49" si="22">U18*180</f>
+        <f t="shared" ref="U49:W49" si="22">U18*180</f>
         <v>3.857526</v>
       </c>
       <c r="V49" s="1"/>
@@ -2574,7 +2574,7 @@
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1">
-        <f t="shared" ref="F50:L50" si="24">G19*180</f>
+        <f t="shared" ref="G50:L50" si="24">G19*180</f>
         <v>6.2167500000000001E-3</v>
       </c>
       <c r="H50" s="1">
@@ -2600,7 +2600,7 @@
       </c>
       <c r="N50" s="1"/>
       <c r="O50" s="1">
-        <f t="shared" ref="N50:W50" si="26">O19*180</f>
+        <f t="shared" ref="O50:S50" si="26">O19*180</f>
         <v>2.2136039999999999E-2</v>
       </c>
       <c r="P50" s="1">
@@ -2621,7 +2621,7 @@
         <v>0.83451419999999998</v>
       </c>
       <c r="U50" s="1">
-        <f t="shared" ref="U50:Z50" si="28">U19*180</f>
+        <f t="shared" ref="U50:W50" si="28">U19*180</f>
         <v>1.5203159999999998</v>
       </c>
       <c r="V50" s="1"/>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1">
-        <f t="shared" ref="F51:L51" si="30">G20*180</f>
+        <f t="shared" ref="G51:L51" si="30">G20*180</f>
         <v>0.19975859999999998</v>
       </c>
       <c r="H51" s="1">
@@ -2682,7 +2682,7 @@
       </c>
       <c r="N51" s="1"/>
       <c r="O51" s="1">
-        <f t="shared" ref="N51:W51" si="32">O20*180</f>
+        <f t="shared" ref="O51:S51" si="32">O20*180</f>
         <v>4.8830039999999998E-3</v>
       </c>
       <c r="P51" s="1">
@@ -2703,7 +2703,7 @@
         <v>3.8180519999999998</v>
       </c>
       <c r="U51" s="1">
-        <f t="shared" ref="U51:Z51" si="34">U20*180</f>
+        <f t="shared" ref="U51:W51" si="34">U20*180</f>
         <v>1.260459</v>
       </c>
       <c r="V51" s="1"/>
@@ -2738,7 +2738,7 @@
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1">
-        <f t="shared" ref="F52:L52" si="36">G21*180</f>
+        <f t="shared" ref="G52:L52" si="36">G21*180</f>
         <v>0.19714139999999999</v>
       </c>
       <c r="H52" s="1">
@@ -2764,7 +2764,7 @@
       </c>
       <c r="N52" s="1"/>
       <c r="O52" s="1">
-        <f t="shared" ref="N52:W52" si="38">O21*180</f>
+        <f t="shared" ref="O52:S52" si="38">O21*180</f>
         <v>3.8764080000000002E-5</v>
       </c>
       <c r="P52" s="1">
@@ -2785,7 +2785,7 @@
         <v>1.903356</v>
       </c>
       <c r="U52" s="1">
-        <f t="shared" ref="U52:Z52" si="40">U21*180</f>
+        <f t="shared" ref="U52:W52" si="40">U21*180</f>
         <v>1.6143785999999998</v>
       </c>
       <c r="V52" s="1"/>
@@ -2820,7 +2820,7 @@
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1">
-        <f t="shared" ref="F53:L53" si="42">G22*180</f>
+        <f t="shared" ref="G53:L53" si="42">G22*180</f>
         <v>1.0041983999999999E-5</v>
       </c>
       <c r="H53" s="1">
@@ -2846,7 +2846,7 @@
       </c>
       <c r="N53" s="1"/>
       <c r="O53" s="1">
-        <f t="shared" ref="N53:W53" si="44">O22*180</f>
+        <f t="shared" ref="O53:S53" si="44">O22*180</f>
         <v>2.0424779999999998E-7</v>
       </c>
       <c r="P53" s="1">
@@ -2867,7 +2867,7 @@
         <v>1.2575429999999999</v>
       </c>
       <c r="U53" s="1">
-        <f t="shared" ref="U53:Z53" si="46">U22*180</f>
+        <f t="shared" ref="U53:W53" si="46">U22*180</f>
         <v>0.9731322</v>
       </c>
       <c r="V53" s="1"/>
@@ -2902,7 +2902,7 @@
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1">
-        <f t="shared" ref="F54:L54" si="48">G23*180</f>
+        <f t="shared" ref="G54:L54" si="48">G23*180</f>
         <v>2.1562020000000001E-2</v>
       </c>
       <c r="H54" s="1">
@@ -2928,7 +2928,7 @@
       </c>
       <c r="N54" s="1"/>
       <c r="O54" s="1">
-        <f t="shared" ref="N54:W54" si="50">O23*180</f>
+        <f t="shared" ref="O54:S54" si="50">O23*180</f>
         <v>0.33769979999999999</v>
       </c>
       <c r="P54" s="1">
@@ -2949,7 +2949,7 @@
         <v>1.0304514</v>
       </c>
       <c r="U54" s="1">
-        <f t="shared" ref="U54:Z54" si="52">U23*180</f>
+        <f t="shared" ref="U54:W54" si="52">U23*180</f>
         <v>3.973176</v>
       </c>
       <c r="V54" s="1"/>
@@ -2984,7 +2984,7 @@
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1">
-        <f t="shared" ref="F55:L55" si="54">G24*180</f>
+        <f t="shared" ref="G55:L55" si="54">G24*180</f>
         <v>0.87998940000000003</v>
       </c>
       <c r="H55" s="1">
@@ -3010,7 +3010,7 @@
       </c>
       <c r="N55" s="1"/>
       <c r="O55" s="1">
-        <f t="shared" ref="N55:W55" si="56">O24*180</f>
+        <f t="shared" ref="O55:S55" si="56">O24*180</f>
         <v>7.3786499999999996E-5</v>
       </c>
       <c r="P55" s="1">
@@ -3031,7 +3031,7 @@
         <v>2.4551460000000001</v>
       </c>
       <c r="U55" s="1">
-        <f t="shared" ref="U55:Z55" si="58">U24*180</f>
+        <f t="shared" ref="U55:W55" si="58">U24*180</f>
         <v>3.4102800000000002</v>
       </c>
       <c r="V55" s="1"/>
@@ -3066,7 +3066,7 @@
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1">
-        <f t="shared" ref="F56:L56" si="60">G25*180</f>
+        <f t="shared" ref="G56:L56" si="60">G25*180</f>
         <v>1.8631440000000001</v>
       </c>
       <c r="H56" s="1">
@@ -3092,7 +3092,7 @@
       </c>
       <c r="N56" s="1"/>
       <c r="O56" s="1">
-        <f t="shared" ref="N56:W56" si="62">O25*180</f>
+        <f t="shared" ref="O56:S56" si="62">O25*180</f>
         <v>1.0974168000000001E-2</v>
       </c>
       <c r="P56" s="1">
@@ -3113,7 +3113,7 @@
         <v>4.8702059999999996</v>
       </c>
       <c r="U56" s="1">
-        <f t="shared" ref="U56:Z56" si="64">U25*180</f>
+        <f t="shared" ref="U56:W56" si="64">U25*180</f>
         <v>1.5377921999999999</v>
       </c>
       <c r="V56" s="1"/>
@@ -3214,7 +3214,7 @@
         <v>0.24754239180000001</v>
       </c>
       <c r="D73" s="1">
-        <f t="shared" ref="D73:I73" si="66">AVERAGE(D47:D56)</f>
+        <f t="shared" ref="D73:E73" si="66">AVERAGE(D47:D56)</f>
         <v>1.2322834199999999</v>
       </c>
       <c r="E73" s="1">
@@ -3236,7 +3236,7 @@
       </c>
       <c r="J73" s="1"/>
       <c r="K73" s="1">
-        <f t="shared" ref="J73:S73" si="68">AVERAGE(K47:K56)</f>
+        <f t="shared" ref="K73:S73" si="68">AVERAGE(K47:K56)</f>
         <v>0.18417429250477019</v>
       </c>
       <c r="L73" s="1">
@@ -3266,7 +3266,7 @@
         <v>0.59497052973839992</v>
       </c>
       <c r="T73" s="1">
-        <f t="shared" ref="T73:V73" si="69">AVERAGE(T47:T56)</f>
+        <f t="shared" ref="T73:U73" si="69">AVERAGE(T47:T56)</f>
         <v>2.3177989800000001</v>
       </c>
       <c r="U73" s="1">
@@ -3296,7 +3296,7 @@
         <v>0.25101165429320771</v>
       </c>
       <c r="D74">
-        <f t="shared" ref="D74:I74" si="71">_xlfn.STDEV.S(D47:D56)</f>
+        <f t="shared" ref="D74:E74" si="71">_xlfn.STDEV.S(D47:D56)</f>
         <v>0.78445209414837025</v>
       </c>
       <c r="E74">
@@ -3316,7 +3316,7 @@
         <v>0.73538780367365142</v>
       </c>
       <c r="K74">
-        <f t="shared" ref="J74:S74" si="73">_xlfn.STDEV.S(K47:K56)</f>
+        <f t="shared" ref="K74:S74" si="73">_xlfn.STDEV.S(K47:K56)</f>
         <v>0.22087721645556738</v>
       </c>
       <c r="L74">
@@ -3344,7 +3344,7 @@
         <v>0.61596199655174544</v>
       </c>
       <c r="T74">
-        <f t="shared" ref="T74:V74" si="74">_xlfn.STDEV.S(T47:T56)</f>
+        <f t="shared" ref="T74:U74" si="74">_xlfn.STDEV.S(T47:T56)</f>
         <v>1.4144738554931318</v>
       </c>
       <c r="U74">

</xml_diff>